<commit_message>
Update uitgaves en testplan
</commit_message>
<xml_diff>
--- a/Opleverset/Extra documenten/Excel sheets/Uitgaves_Floating_Farm.xlsx
+++ b/Opleverset/Extra documenten/Excel sheets/Uitgaves_Floating_Farm.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mrtha\Documents\GitHub\Project-5-6---Floating-Farm\Opleverset\Extra documenten\Excel sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61121542-C572-496A-B0A1-74F60C1A99AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07B33E84-386C-4146-AA64-862A9864B8D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{14AEBCC3-6D87-4B1A-9D64-0CD8C4A83626}"/>
+    <workbookView xWindow="2660" yWindow="2660" windowWidth="19200" windowHeight="11170" xr2:uid="{14AEBCC3-6D87-4B1A-9D64-0CD8C4A83626}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Item</t>
   </si>
@@ -77,13 +77,25 @@
     <t>4x DC connector male adapters</t>
   </si>
   <si>
-    <t>geprojecteerde prijzen:</t>
-  </si>
-  <si>
     <t>QBOARD boardfix montage lijm 290 ml</t>
   </si>
   <si>
     <t>QBOARD BASIQ Bouwplaat 1200mm x 600mm</t>
+  </si>
+  <si>
+    <t>Opbergbox voor demonstratie</t>
+  </si>
+  <si>
+    <t>Afdekfolie 4x5m</t>
+  </si>
+  <si>
+    <t>Houten plaat, prototype 2</t>
+  </si>
+  <si>
+    <t>Arcylplaat 25x50cm</t>
+  </si>
+  <si>
+    <t>concept uitgaves</t>
   </si>
 </sst>
 </file>
@@ -461,10 +473,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68DF2FA7-E7C3-4436-AF28-B59F61D87239}">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -473,9 +485,10 @@
     <col min="2" max="2" width="8.6328125" customWidth="1"/>
     <col min="3" max="3" width="17.1796875" customWidth="1"/>
     <col min="4" max="4" width="10.08984375" customWidth="1"/>
+    <col min="8" max="8" width="37.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -489,7 +502,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -501,10 +514,13 @@
       </c>
       <c r="E2" s="1">
         <f>SUM(B2:B1048576)</f>
-        <v>83.38</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+        <v>78.490000000000009</v>
+      </c>
+      <c r="H2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -515,23 +531,35 @@
         <v>45758</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>7</v>
       </c>
       <c r="B4">
         <v>4.95</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="H4" t="s">
+        <v>14</v>
+      </c>
+      <c r="I4">
+        <v>13.45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>8</v>
       </c>
       <c r="B5">
         <v>12.41</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="H5" t="s">
+        <v>13</v>
+      </c>
+      <c r="I5">
+        <v>12.91</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -539,7 +567,7 @@
         <v>3.11</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -547,7 +575,7 @@
         <v>6.99</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -555,7 +583,7 @@
         <v>1.49</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -563,25 +591,36 @@
         <v>1.61</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10">
+        <v>3.82</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+        <v>16</v>
+      </c>
+      <c r="B11">
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B12">
-        <v>13.45</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B13">
-        <v>12.91</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>